<commit_message>
ADded python for placeholder to parse xlsl to csv for now
</commit_message>
<xml_diff>
--- a/Mir/External/testdata/testdata.xlsx
+++ b/Mir/External/testdata/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35850\Desktop\repositories\learning2\Learning\Mir\External\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219CC766-D749-4DA3-AB48-190FF51D8F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4DF8AB-3C94-404C-B29F-DD600D00862B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="2010" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -386,7 +387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -484,4 +485,35 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B9B3D8-FBF4-4B07-9A30-9B7BE37996F4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>41234</v>
+      </c>
+      <c r="B1">
+        <v>2131321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1321</v>
+      </c>
+      <c r="B2">
+        <v>321312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
READ from csv -> save to .typ file working. with std::map implementation
</commit_message>
<xml_diff>
--- a/Mir/External/testdata/testdata.xlsx
+++ b/Mir/External/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35850\Desktop\repositories\learning2\Learning\Mir\External\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4DF8AB-3C94-404C-B29F-DD600D00862B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9B4125-0E2D-4F1A-B1E2-12C336D9FFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="2010" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>AF101</t>
   </si>
@@ -37,9 +37,6 @@
     <t>IOCARD</t>
   </si>
   <si>
-    <t>DI</t>
-  </si>
-  <si>
     <t>DEVICE</t>
   </si>
   <si>
@@ -62,6 +59,39 @@
   </si>
   <si>
     <t>pump7</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>NO COMMENT</t>
+  </si>
+  <si>
+    <t>AF102</t>
+  </si>
+  <si>
+    <t>TATU</t>
+  </si>
+  <si>
+    <t>SAMI</t>
+  </si>
+  <si>
+    <t>TEEMU</t>
+  </si>
+  <si>
+    <t>VICE</t>
+  </si>
+  <si>
+    <t>SMILEY</t>
+  </si>
+  <si>
+    <t>TIPZU</t>
+  </si>
+  <si>
+    <t>FINU</t>
+  </si>
+  <si>
+    <t>BOOL</t>
   </si>
 </sst>
 </file>
@@ -385,17 +415,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -403,82 +436,204 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -491,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B9B3D8-FBF4-4B07-9A30-9B7BE37996F4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>